<commit_message>
Updated formatting and moved old files to archive
</commit_message>
<xml_diff>
--- a/Test Case - 1/TC1Results_B.xlsx
+++ b/Test Case - 1/TC1Results_B.xlsx
@@ -830,7 +830,27 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -848,6 +868,76 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1235,8 +1325,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1375,14 +1465,6 @@
       <c r="O3" t="b">
         <v>1</v>
       </c>
-      <c r="S3" t="e">
-        <f>0.9*((R3-D3)^0.51)*((SQRT((P3-B3)^2+(Q3-C3)^2)^(-0.35)))</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="T3" t="e">
-        <f>IF(M3=0,TRUE,OR(AND(S3&lt;(M3*1.03),S3&gt;(M3*0.97)),O3))</f>
-        <v>#NUM!</v>
-      </c>
       <c r="V3">
         <f>IF(K3=TRUE,1,0)</f>
         <v>1</v>
@@ -1443,16 +1525,8 @@
       <c r="R4">
         <v>20.152000000000001</v>
       </c>
-      <c r="S4">
-        <f t="shared" ref="S4:S23" si="0">0.9*((R4-D4)^0.51)*((SQRT((P4-B4)^2+(Q4-C4)^2)^(-0.35)))</f>
-        <v>1.0214234395596546</v>
-      </c>
-      <c r="T4" t="b">
-        <f t="shared" ref="T4:T23" si="1">IF(M4=0,TRUE,OR(AND(S4&lt;(M4*1.03),S4&gt;(M4*0.97)),O4))</f>
-        <v>1</v>
-      </c>
       <c r="V4">
-        <f t="shared" ref="V4:V53" si="2">IF(K4=TRUE,1,0)</f>
+        <f t="shared" ref="V4:V53" si="0">IF(K4=TRUE,1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -1511,16 +1585,8 @@
       <c r="R5">
         <v>20.152000000000001</v>
       </c>
-      <c r="S5">
-        <f t="shared" si="0"/>
-        <v>1.0211781152081296</v>
-      </c>
-      <c r="T5" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
       <c r="V5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1580,15 +1646,15 @@
         <v>20.152000000000001</v>
       </c>
       <c r="S6">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="S4:S23" si="1">0.9*((R6-D6)^0.51)*((SQRT((P6-B6)^2+(Q6-C6)^2)^(-0.35)))</f>
         <v>1.6044811859611072</v>
       </c>
       <c r="T6" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="T4:T23" si="2">IF(M6=0,TRUE,OR(AND(S6&lt;(M6*1.03),S6&gt;(M6*0.97)),O6))</f>
         <v>1</v>
       </c>
       <c r="V6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1647,16 +1713,8 @@
       <c r="R7">
         <v>20.152000000000001</v>
       </c>
-      <c r="S7">
-        <f t="shared" si="0"/>
-        <v>1.6596977981112069</v>
-      </c>
-      <c r="T7" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
       <c r="V7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1716,15 +1774,15 @@
         <v>30.152000000000001</v>
       </c>
       <c r="S8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.8572810214170183</v>
       </c>
       <c r="T8" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="V8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1784,15 +1842,15 @@
         <v>30.152000000000001</v>
       </c>
       <c r="S9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.3300018437466941</v>
       </c>
       <c r="T9" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="V9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1851,16 +1909,8 @@
       <c r="R10">
         <v>30.152000000000001</v>
       </c>
-      <c r="S10">
-        <f t="shared" si="0"/>
-        <v>1.3017612596028523</v>
-      </c>
-      <c r="T10" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
       <c r="V10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1919,16 +1969,8 @@
       <c r="R11">
         <v>30.152000000000001</v>
       </c>
-      <c r="S11">
-        <f t="shared" si="0"/>
-        <v>1.3100375076613813</v>
-      </c>
-      <c r="T11" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
       <c r="V11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1987,16 +2029,8 @@
       <c r="R12">
         <v>30.152000000000001</v>
       </c>
-      <c r="S12">
-        <f t="shared" si="0"/>
-        <v>1.1693623831592181</v>
-      </c>
-      <c r="T12" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
       <c r="V12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2055,16 +2089,8 @@
       <c r="R13">
         <v>30.152000000000001</v>
       </c>
-      <c r="S13">
-        <f t="shared" si="0"/>
-        <v>1.1693700515158973</v>
-      </c>
-      <c r="T13" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
       <c r="V13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2123,16 +2149,8 @@
       <c r="R14">
         <v>30.152000000000001</v>
       </c>
-      <c r="S14">
-        <f t="shared" si="0"/>
-        <v>1.2285568778866769</v>
-      </c>
-      <c r="T14" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
       <c r="V14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2192,15 +2210,15 @@
         <v>30.152000000000001</v>
       </c>
       <c r="S15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.2817510033089079</v>
       </c>
       <c r="T15" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="V15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2259,16 +2277,8 @@
       <c r="R16">
         <v>30.152000000000001</v>
       </c>
-      <c r="S16">
-        <f t="shared" si="0"/>
-        <v>1.3107091227591259</v>
-      </c>
-      <c r="T16" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
       <c r="V16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2327,16 +2337,8 @@
       <c r="R17">
         <v>30.152000000000001</v>
       </c>
-      <c r="S17">
-        <f t="shared" si="0"/>
-        <v>1.3008956092694441</v>
-      </c>
-      <c r="T17" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
       <c r="V17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2396,15 +2398,15 @@
         <v>30.152000000000001</v>
       </c>
       <c r="S18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5084318657314502</v>
       </c>
       <c r="T18" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="V18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2463,16 +2465,8 @@
       <c r="R19">
         <v>30.152000000000001</v>
       </c>
-      <c r="S19">
-        <f t="shared" si="0"/>
-        <v>1.3016662910134993</v>
-      </c>
-      <c r="T19" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
       <c r="V19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2531,16 +2525,8 @@
       <c r="R20">
         <v>30.152000000000001</v>
       </c>
-      <c r="S20">
-        <f t="shared" si="0"/>
-        <v>1.3100662617195269</v>
-      </c>
-      <c r="T20" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
       <c r="V20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2599,16 +2585,8 @@
       <c r="R21">
         <v>30.152000000000001</v>
       </c>
-      <c r="S21">
-        <f t="shared" si="0"/>
-        <v>1.1524324040824301</v>
-      </c>
-      <c r="T21" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
       <c r="V21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2667,16 +2645,8 @@
       <c r="R22">
         <v>30.152000000000001</v>
       </c>
-      <c r="S22">
-        <f t="shared" si="0"/>
-        <v>1.3100662617195269</v>
-      </c>
-      <c r="T22" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
       <c r="V22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2735,16 +2705,8 @@
       <c r="R23">
         <v>30.152000000000001</v>
       </c>
-      <c r="S23">
-        <f t="shared" si="0"/>
-        <v>1.3011674305281238</v>
-      </c>
-      <c r="T23" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
       <c r="V23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2812,7 +2774,7 @@
         <v>1</v>
       </c>
       <c r="V24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2871,16 +2833,8 @@
       <c r="R25">
         <v>30.152000000000001</v>
       </c>
-      <c r="S25">
-        <f t="shared" si="3"/>
-        <v>1.3004407781547296</v>
-      </c>
-      <c r="T25" t="b">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
       <c r="V25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2939,16 +2893,8 @@
       <c r="R26">
         <v>30.152000000000001</v>
       </c>
-      <c r="S26">
-        <f t="shared" si="3"/>
-        <v>1.1523718606121613</v>
-      </c>
-      <c r="T26" t="b">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
       <c r="V26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3007,16 +2953,8 @@
       <c r="R27">
         <v>30.152000000000001</v>
       </c>
-      <c r="S27">
-        <f t="shared" si="3"/>
-        <v>1.3100310682100755</v>
-      </c>
-      <c r="T27" t="b">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
       <c r="V27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3075,16 +3013,8 @@
       <c r="R28">
         <v>30.152000000000001</v>
       </c>
-      <c r="S28">
-        <f t="shared" si="3"/>
-        <v>1.3011234156165259</v>
-      </c>
-      <c r="T28" t="b">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
       <c r="V28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3143,16 +3073,8 @@
       <c r="R29">
         <v>30.152000000000001</v>
       </c>
-      <c r="S29">
-        <f t="shared" si="3"/>
-        <v>1.6595797676713377</v>
-      </c>
-      <c r="T29" t="b">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
       <c r="V29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3199,16 +3121,8 @@
       <c r="O30" t="b">
         <v>1</v>
       </c>
-      <c r="S30" t="e">
-        <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="T30" t="e">
-        <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
       <c r="V30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3255,16 +3169,8 @@
       <c r="O31" t="b">
         <v>1</v>
       </c>
-      <c r="S31" t="e">
-        <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="T31" t="e">
-        <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
       <c r="V31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3311,16 +3217,8 @@
       <c r="O32" t="b">
         <v>1</v>
       </c>
-      <c r="S32" t="e">
-        <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="T32" t="e">
-        <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
       <c r="V32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3367,16 +3265,8 @@
       <c r="O33" t="b">
         <v>1</v>
       </c>
-      <c r="S33" t="e">
-        <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="T33" t="e">
-        <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
       <c r="V33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3423,16 +3313,8 @@
       <c r="O34" t="b">
         <v>1</v>
       </c>
-      <c r="S34" t="e">
-        <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="T34" t="e">
-        <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
       <c r="V34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3479,16 +3361,8 @@
       <c r="O35" t="b">
         <v>1</v>
       </c>
-      <c r="S35" t="e">
-        <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="T35" t="e">
-        <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
       <c r="V35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3535,16 +3409,8 @@
       <c r="O36" t="b">
         <v>1</v>
       </c>
-      <c r="S36" t="e">
-        <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="T36" t="e">
-        <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
       <c r="V36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3591,16 +3457,8 @@
       <c r="O37" t="b">
         <v>1</v>
       </c>
-      <c r="S37" t="e">
-        <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="T37" t="e">
-        <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
       <c r="V37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3647,16 +3505,8 @@
       <c r="O38" t="b">
         <v>1</v>
       </c>
-      <c r="S38" t="e">
-        <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="T38" t="e">
-        <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
       <c r="V38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3703,16 +3553,8 @@
       <c r="O39" t="b">
         <v>1</v>
       </c>
-      <c r="S39" t="e">
-        <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="T39" t="e">
-        <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
       <c r="V39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3759,16 +3601,8 @@
       <c r="O40" t="b">
         <v>1</v>
       </c>
-      <c r="S40" t="e">
-        <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="T40" t="e">
-        <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
       <c r="V40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3815,16 +3649,8 @@
       <c r="O41" t="b">
         <v>1</v>
       </c>
-      <c r="S41" t="e">
-        <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="T41" t="e">
-        <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
       <c r="V41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3871,16 +3697,8 @@
       <c r="O42" t="b">
         <v>1</v>
       </c>
-      <c r="S42" t="e">
-        <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="T42" t="e">
-        <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
       <c r="V42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3927,16 +3745,8 @@
       <c r="O43" t="b">
         <v>1</v>
       </c>
-      <c r="S43" t="e">
-        <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="T43" t="e">
-        <f t="shared" si="4"/>
-        <v>#NUM!</v>
-      </c>
       <c r="V43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3983,16 +3793,8 @@
       <c r="O44" t="b">
         <v>1</v>
       </c>
-      <c r="S44" t="e">
-        <f t="shared" ref="S44:S53" si="5">0.9*((R44-D44)^0.51)*((SQRT((P44-B44)^2+(Q44-C44)^2)^(-0.35)))</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="T44" t="e">
-        <f t="shared" ref="T44:T53" si="6">IF(M44=0,TRUE,OR(AND(S44&lt;(M44*1.03),S44&gt;(M44*0.97)),O44))</f>
-        <v>#NUM!</v>
-      </c>
       <c r="V44">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4039,16 +3841,8 @@
       <c r="O45" t="b">
         <v>1</v>
       </c>
-      <c r="S45" t="e">
-        <f t="shared" si="5"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="T45" t="e">
-        <f t="shared" si="6"/>
-        <v>#NUM!</v>
-      </c>
       <c r="V45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4095,16 +3889,8 @@
       <c r="O46" t="b">
         <v>1</v>
       </c>
-      <c r="S46" t="e">
-        <f t="shared" si="5"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="T46" t="e">
-        <f t="shared" si="6"/>
-        <v>#NUM!</v>
-      </c>
       <c r="V46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4151,16 +3937,8 @@
       <c r="O47" t="b">
         <v>1</v>
       </c>
-      <c r="S47" t="e">
-        <f t="shared" si="5"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="T47" t="e">
-        <f t="shared" si="6"/>
-        <v>#NUM!</v>
-      </c>
       <c r="V47">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4207,16 +3985,8 @@
       <c r="O48" t="b">
         <v>1</v>
       </c>
-      <c r="S48" t="e">
-        <f t="shared" si="5"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="T48" t="e">
-        <f t="shared" si="6"/>
-        <v>#NUM!</v>
-      </c>
       <c r="V48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4263,16 +4033,8 @@
       <c r="O49" t="b">
         <v>1</v>
       </c>
-      <c r="S49" t="e">
-        <f t="shared" si="5"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="T49" t="e">
-        <f t="shared" si="6"/>
-        <v>#NUM!</v>
-      </c>
       <c r="V49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4319,16 +4081,8 @@
       <c r="O50" t="b">
         <v>1</v>
       </c>
-      <c r="S50" t="e">
-        <f t="shared" si="5"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="T50" t="e">
-        <f t="shared" si="6"/>
-        <v>#NUM!</v>
-      </c>
       <c r="V50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -4375,16 +4129,8 @@
       <c r="O51" t="b">
         <v>1</v>
       </c>
-      <c r="S51" t="e">
-        <f t="shared" si="5"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="T51" t="e">
-        <f t="shared" si="6"/>
-        <v>#NUM!</v>
-      </c>
       <c r="V51">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4431,16 +4177,8 @@
       <c r="O52" t="b">
         <v>1</v>
       </c>
-      <c r="S52" t="e">
-        <f t="shared" si="5"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="T52" t="e">
-        <f t="shared" si="6"/>
-        <v>#NUM!</v>
-      </c>
       <c r="V52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4487,16 +4225,8 @@
       <c r="O53" t="b">
         <v>1</v>
       </c>
-      <c r="S53" t="e">
-        <f t="shared" si="5"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="T53" t="e">
-        <f t="shared" si="6"/>
-        <v>#NUM!</v>
-      </c>
       <c r="V53">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4593,11 +4323,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="N1:N2"/>
-    <mergeCell ref="O1:O2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
@@ -4608,13 +4333,28 @@
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:J2"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="O1:O2"/>
   </mergeCells>
-  <conditionalFormatting sqref="K58 O58 T58 K3:K53 O3:O53 T3:T53">
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+  <conditionalFormatting sqref="K58 O58 T58 K3:K53 O3:O53">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:K53">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O3:O53">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T3:T53">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>

</xml_diff>